<commit_message>
terminado primeiro esboço das APIs
</commit_message>
<xml_diff>
--- a/FPGA_Developments/COM_Module_v1_5/References/NIOS_COMM_v1.5_Map.xlsx
+++ b/FPGA_Developments/COM_Module_v1_5/References/NIOS_COMM_v1.5_Map.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfranca\Dev\SimuCam_Development\FPGA_Developments\COM_Module_v1_5\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0235F7AD-4CF1-470B-BCE0-E4BC6C47C18A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D411AF03-26BA-4AAB-A854-80FA185261C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11628" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVS COMM Registers Named" sheetId="1" r:id="rId1"/>
     <sheet name="AVS COMM Registers" sheetId="17" r:id="rId2"/>
     <sheet name="AVS COMM Registers TABLE" sheetId="13" r:id="rId3"/>
-    <sheet name="Register VHDL Types" sheetId="14" r:id="rId4"/>
-    <sheet name="Register VHDL Types TABLE" sheetId="18" r:id="rId5"/>
-    <sheet name="Register VHDL RMAP RD Case" sheetId="15" r:id="rId6"/>
-    <sheet name="Register VHDL RMAP WR Case" sheetId="16" r:id="rId7"/>
+    <sheet name="NIOS defines" sheetId="19" r:id="rId4"/>
+    <sheet name="Register VHDL Types" sheetId="14" r:id="rId5"/>
+    <sheet name="Register VHDL Types TABLE" sheetId="18" r:id="rId6"/>
+    <sheet name="Register VHDL RMAP RD Case" sheetId="15" r:id="rId7"/>
+    <sheet name="Register VHDL RMAP WR Case" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5284" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="358">
   <si>
     <t>Address</t>
   </si>
@@ -821,12 +822,303 @@
   <si>
     <t>rmap_err_header_crc</t>
   </si>
+  <si>
+    <t>Define name</t>
+  </si>
+  <si>
+    <t>Full Define</t>
+  </si>
+  <si>
+    <t>Addr [hex]</t>
+  </si>
+  <si>
+    <t>Define suffix</t>
+  </si>
+  <si>
+    <t>Define prefix</t>
+  </si>
+  <si>
+    <t>COMM_</t>
+  </si>
+  <si>
+    <t>Name length</t>
+  </si>
+  <si>
+    <t>TIMECODE</t>
+  </si>
+  <si>
+    <t>LINK_CFG_STAT</t>
+  </si>
+  <si>
+    <t>FEE_BUFF_CFG</t>
+  </si>
+  <si>
+    <t>FEE_BUFF_STAT</t>
+  </si>
+  <si>
+    <t>RMAP_CODEC_STAT</t>
+  </si>
+  <si>
+    <t>RMAP_CODEC_CFG</t>
+  </si>
+  <si>
+    <t>RMAP_LST_WR_ADDR</t>
+  </si>
+  <si>
+    <t>_REG_OFST</t>
+  </si>
+  <si>
+    <t>RMAP_LST_RD_ADDR</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CFG_1</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CFG_2</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CFG_3</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CFG_4</t>
+  </si>
+  <si>
+    <t>DATA_PKT_HDR_1</t>
+  </si>
+  <si>
+    <t>DATA_PKT_HDR_2</t>
+  </si>
+  <si>
+    <t>DATA_PKT_PX_DLY_1</t>
+  </si>
+  <si>
+    <t>DATA_PKT_PX_DLY_2</t>
+  </si>
+  <si>
+    <t>DATA_PKT_PX_DLY_3</t>
+  </si>
+  <si>
+    <t>IRQ_CONTROL</t>
+  </si>
+  <si>
+    <t>IRQ_FLAGS</t>
+  </si>
+  <si>
+    <t>IRQ_FLAGS_CLR</t>
+  </si>
+  <si>
+    <t>Final Text</t>
+  </si>
+  <si>
+    <t>Bit Mask Name</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>0b111111</t>
+  </si>
+  <si>
+    <t>0b11</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>_MSK</t>
+  </si>
+  <si>
+    <t>SPW_LNKCFG_DISCONNECT</t>
+  </si>
+  <si>
+    <t>SPW_LNKCFG_LINKSTART</t>
+  </si>
+  <si>
+    <t>SPW_LNKCFG_AUTOSTART</t>
+  </si>
+  <si>
+    <t>SPW_LNKERR_DISCONNECT</t>
+  </si>
+  <si>
+    <t>SPW_LNKSTAT_RUNNING</t>
+  </si>
+  <si>
+    <t>SPW_LNKSTAT_CONNECTING</t>
+  </si>
+  <si>
+    <t>SPW_LNKSTAT_STARTED</t>
+  </si>
+  <si>
+    <t>SPW_LNKERR_PARITY</t>
+  </si>
+  <si>
+    <t>SPW_LNKERR_ESCAPE</t>
+  </si>
+  <si>
+    <t>SPW_LNKERR_CREDIT</t>
+  </si>
+  <si>
+    <t>SPW_LNKCFG_TXDIVCNT</t>
+  </si>
+  <si>
+    <t>TIMECODE_TIME</t>
+  </si>
+  <si>
+    <t>TIMECODE_CONTROL</t>
+  </si>
+  <si>
+    <t>FEE_MACHINE_CLR</t>
+  </si>
+  <si>
+    <t>TIMECODE_CLR</t>
+  </si>
+  <si>
+    <t>FEE_MACHINE_STOP</t>
+  </si>
+  <si>
+    <t>FEE_MACHINE_START</t>
+  </si>
+  <si>
+    <t>FEE_MASKING_EN</t>
+  </si>
+  <si>
+    <t>WIND_RIGH_BUFF_EMPTY</t>
+  </si>
+  <si>
+    <t>WIND_LEFT_BUFF_EMPTY</t>
+  </si>
+  <si>
+    <t>RMAP_TARGET_LOG_ADDR</t>
+  </si>
+  <si>
+    <t>RMAP_TARGET_KEY</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_CMD_RECEIVED</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_WR_AUTH</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_WR_REQ</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_RD_REQ</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_RD_AUTH</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_REPLY_SEND</t>
+  </si>
+  <si>
+    <t>RMAP_STAT_DISCARD_PKG</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_EARLY_EOP</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_EEP</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_HEADER_CRC</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_UNUSED_PKT</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_INVALID_CMD</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_TOO_MUCH_DATA</t>
+  </si>
+  <si>
+    <t>RMAP_ERR_INVALID_DCRC</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CCD_X_SIZE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CCD_Y_SIZE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_DATA_Y_SIZE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_OVER_Y_SIZE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_LENGTH</t>
+  </si>
+  <si>
+    <t>DATA_PKT_FEE_MODE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_CCD_NUMBER</t>
+  </si>
+  <si>
+    <t>DATA_PKT_HDR_LENGTH</t>
+  </si>
+  <si>
+    <t>DATA_PKT_HDR_TYPE</t>
+  </si>
+  <si>
+    <t>DATA_PKT_HDR_FRAME_CNT</t>
+  </si>
+  <si>
+    <t>DATA_PKT_SEQ_CNT</t>
+  </si>
+  <si>
+    <t>DATA_PKT_LINE_DLY</t>
+  </si>
+  <si>
+    <t>DATA_PKT_COLUMN_DLY</t>
+  </si>
+  <si>
+    <t>DATA_PKT_ADC_DLY</t>
+  </si>
+  <si>
+    <t>IRQ_RIGH_BUFF_EPY_EN</t>
+  </si>
+  <si>
+    <t>IRQ_LEFT_BUFF_EPY_EN</t>
+  </si>
+  <si>
+    <t>IRQ_GLOBAL_EN</t>
+  </si>
+  <si>
+    <t>IRQ_BUFF_EPY_FLG_CLR</t>
+  </si>
+  <si>
+    <t>IRQ_RMAP_WRCMD_FLG_CLR</t>
+  </si>
+  <si>
+    <t>IRQ_BUFF_EPY_FLG</t>
+  </si>
+  <si>
+    <t>IRQ_RMAP_WRCMD_FLG</t>
+  </si>
+  <si>
+    <t>IRQ_RMAP_WRCMD_EN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,6 +1169,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1077,7 +1375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1250,6 +1548,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,8 +1834,8 @@
   </sheetPr>
   <dimension ref="A1:AH140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10224,9 +10523,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH140"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22182,6 +22479,3207 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D061FBA-07C0-4F72-BCD6-B54744C5B3B8}">
+  <dimension ref="C2:O103"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="36.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="32" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" style="32" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5546875" style="32" customWidth="1"/>
+    <col min="10" max="11" width="12.109375" style="32" customWidth="1"/>
+    <col min="12" max="12" width="37.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="76" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D3</f>
+        <v>spw_link_config_status_reg</v>
+      </c>
+      <c r="D3" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C3,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x00</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L3" s="32" t="str">
+        <f>CONCATENATE(H3,I3,J3)</f>
+        <v>COMM_LINK_CFG_STAT_REG_OFST</v>
+      </c>
+      <c r="M3" s="32">
+        <f>LEN(L3)</f>
+        <v>27</v>
+      </c>
+      <c r="O3" s="62" t="str">
+        <f>CONCATENATE("#define ",L3, REPT(" ",32 - LEN(L3))," ",D3)</f>
+        <v>#define COMM_LINK_CFG_STAT_REG_OFST      0x00</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D17</f>
+        <v>spw_timecode_reg</v>
+      </c>
+      <c r="D4" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C4,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x01</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L4" s="32" t="str">
+        <f t="shared" ref="L4:L22" si="0">CONCATENATE(H4,I4,J4)</f>
+        <v>COMM_TIMECODE_REG_OFST</v>
+      </c>
+      <c r="M4" s="32">
+        <f t="shared" ref="M4:M22" si="1">LEN(L4)</f>
+        <v>22</v>
+      </c>
+      <c r="O4" s="62" t="str">
+        <f t="shared" ref="O4:O22" si="2">CONCATENATE("#define ",L4, REPT(" ",32 - LEN(L4))," ",D4)</f>
+        <v>#define COMM_TIMECODE_REG_OFST           0x01</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C5" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D21</f>
+        <v>fee_windowing_buffers_config_reg</v>
+      </c>
+      <c r="D5" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C5,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x02</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L5" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_FEE_BUFF_CFG_REG_OFST</v>
+      </c>
+      <c r="M5" s="32">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="O5" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_FEE_BUFF_CFG_REG_OFST       0x02</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D26</f>
+        <v>fee_windowing_buffers_status_reg</v>
+      </c>
+      <c r="D6" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C6,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x03</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L6" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_FEE_BUFF_STAT_REG_OFST</v>
+      </c>
+      <c r="M6" s="32">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="O6" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_FEE_BUFF_STAT_REG_OFST      0x03</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D29</f>
+        <v>rmap_codec_config_reg</v>
+      </c>
+      <c r="D7" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C7,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x04</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L7" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_RMAP_CODEC_CFG_REG_OFST</v>
+      </c>
+      <c r="M7" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O7" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_RMAP_CODEC_CFG_REG_OFST     0x04</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D32</f>
+        <v>rmap_codec_status_reg</v>
+      </c>
+      <c r="D8" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C8,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x05</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L8" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_RMAP_CODEC_STAT_REG_OFST</v>
+      </c>
+      <c r="M8" s="32">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="O8" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_RMAP_CODEC_STAT_REG_OFST    0x05</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C9" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D48</f>
+        <v>rmap_last_write_addr_reg</v>
+      </c>
+      <c r="D9" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C9,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x06</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L9" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_RMAP_LST_WR_ADDR_REG_OFST</v>
+      </c>
+      <c r="M9" s="32">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O9" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_RMAP_LST_WR_ADDR_REG_OFST   0x06</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D49</f>
+        <v>rmap_last_read_addr_reg</v>
+      </c>
+      <c r="D10" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C10,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x07</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L10" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_RMAP_LST_RD_ADDR_REG_OFST</v>
+      </c>
+      <c r="M10" s="32">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O10" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_RMAP_LST_RD_ADDR_REG_OFST   0x07</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D50</f>
+        <v>data_packet_config_1_reg</v>
+      </c>
+      <c r="D11" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C11,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x08</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L11" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_CFG_1_REG_OFST</v>
+      </c>
+      <c r="M11" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O11" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_CFG_1_REG_OFST     0x08</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D52</f>
+        <v>data_packet_config_2_reg</v>
+      </c>
+      <c r="D12" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C12,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x09</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L12" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_CFG_2_REG_OFST</v>
+      </c>
+      <c r="M12" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O12" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_CFG_2_REG_OFST     0x09</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D54</f>
+        <v>data_packet_config_3_reg</v>
+      </c>
+      <c r="D13" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C13,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0A</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L13" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_CFG_3_REG_OFST</v>
+      </c>
+      <c r="M13" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O13" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_CFG_3_REG_OFST     0x0A</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D56</f>
+        <v>data_packet_config_4_reg</v>
+      </c>
+      <c r="D14" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C14,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0B</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L14" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_CFG_4_REG_OFST</v>
+      </c>
+      <c r="M14" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O14" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_CFG_4_REG_OFST     0x0B</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C15" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D59</f>
+        <v>data_packet_header_1_reg</v>
+      </c>
+      <c r="D15" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C15,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0C</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L15" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_HDR_1_REG_OFST</v>
+      </c>
+      <c r="M15" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O15" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_HDR_1_REG_OFST     0x0C</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C16" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D61</f>
+        <v>data_packet_header_2_reg</v>
+      </c>
+      <c r="D16" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C16,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0D</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L16" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_HDR_2_REG_OFST</v>
+      </c>
+      <c r="M16" s="32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O16" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_HDR_2_REG_OFST     0x0D</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D63</f>
+        <v>data_packet_pixel_delay_1_reg</v>
+      </c>
+      <c r="D17" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C17,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L17" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_PX_DLY_1_REG_OFST</v>
+      </c>
+      <c r="M17" s="32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="O17" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_PX_DLY_1_REG_OFST  0x0E</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D65</f>
+        <v>data_packet_pixel_delay_2_reg</v>
+      </c>
+      <c r="D18" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C18,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x0F</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L18" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_PX_DLY_2_REG_OFST</v>
+      </c>
+      <c r="M18" s="32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="O18" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_PX_DLY_2_REG_OFST  0x0F</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D67</f>
+        <v>data_packet_pixel_delay_3_reg</v>
+      </c>
+      <c r="D19" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C19,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x10</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L19" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_DATA_PKT_PX_DLY_3_REG_OFST</v>
+      </c>
+      <c r="M19" s="32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="O19" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_DATA_PKT_PX_DLY_3_REG_OFST  0x10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C20" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D69</f>
+        <v>comm_irq_control_reg</v>
+      </c>
+      <c r="D20" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C20,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x11</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L20" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_IRQ_CONTROL_REG_OFST</v>
+      </c>
+      <c r="M20" s="32">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="O20" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_IRQ_CONTROL_REG_OFST        0x11</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C21" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D76</f>
+        <v>comm_irq_flags_reg</v>
+      </c>
+      <c r="D21" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C21,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x12</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L21" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_IRQ_FLAGS_REG_OFST</v>
+      </c>
+      <c r="M21" s="32">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="O21" s="62" t="str">
+        <f t="shared" si="2"/>
+        <v>#define COMM_IRQ_FLAGS_REG_OFST          0x12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C22" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!D80</f>
+        <v>comm_irq_flags_clear_reg</v>
+      </c>
+      <c r="D22" s="32" t="str">
+        <f>INDEX('AVS COMM Registers TABLE'!$B$2:$B$83,MATCH('NIOS defines'!C22,'AVS COMM Registers TABLE'!$D$2:$D$83,0))</f>
+        <v>0x13</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L22" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>COMM_IRQ_FLAGS_CLR_REG_OFST</v>
+      </c>
+      <c r="M22" s="32">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="O22" s="62" t="str">
+        <f>CONCATENATE("#define ",L22, REPT(" ",32 - LEN(L22))," ",D22)</f>
+        <v>#define COMM_IRQ_FLAGS_CLR_REG_OFST      0x13</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C24" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="M24" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="O24" s="33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E3</f>
+        <v>spw_lnkcfg_disconnect</v>
+      </c>
+      <c r="D25" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C25,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="32">
+        <v>1</v>
+      </c>
+      <c r="F25" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C25,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L25" s="32" t="str">
+        <f t="shared" ref="L25" si="3">CONCATENATE(H25,I25,J25)</f>
+        <v>COMM_SPW_LNKCFG_DISCONNECT_MSK</v>
+      </c>
+      <c r="M25" s="32">
+        <f t="shared" ref="M25:M94" si="4">LEN(L25)</f>
+        <v>30</v>
+      </c>
+      <c r="O25" s="62" t="str">
+        <f>CONCATENATE("#define ",L25, REPT(" ",32 - LEN(L25))," ","(", E25," &lt;&lt; ", F25,")")</f>
+        <v>#define COMM_SPW_LNKCFG_DISCONNECT_MSK   (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C26" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E4</f>
+        <v>spw_lnkcfg_linkstart</v>
+      </c>
+      <c r="D26" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C26,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="32">
+        <v>1</v>
+      </c>
+      <c r="F26" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C26,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L26" s="32" t="str">
+        <f t="shared" ref="L26:L35" si="5">CONCATENATE(H26,I26,J26)</f>
+        <v>COMM_SPW_LNKCFG_LINKSTART_MSK</v>
+      </c>
+      <c r="M26" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O26" s="62" t="str">
+        <f t="shared" ref="O26:O94" si="6">CONCATENATE("#define ",L26, REPT(" ",32 - LEN(L26))," ","(", E26," &lt;&lt; ", F26,")")</f>
+        <v>#define COMM_SPW_LNKCFG_LINKSTART_MSK    (1 &lt;&lt; 1)</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C27" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E5</f>
+        <v>spw_lnkcfg_autostart</v>
+      </c>
+      <c r="D27" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C27,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <v>1</v>
+      </c>
+      <c r="F27" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C27,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>2</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L27" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKCFG_AUTOSTART_MSK</v>
+      </c>
+      <c r="M27" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O27" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKCFG_AUTOSTART_MSK    (1 &lt;&lt; 2)</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C28" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E7</f>
+        <v>spw_link_running</v>
+      </c>
+      <c r="D28" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C28,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <v>1</v>
+      </c>
+      <c r="F28" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C28,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L28" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKSTAT_RUNNING_MSK</v>
+      </c>
+      <c r="M28" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKSTAT_RUNNING_MSK     (1 &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C29" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E8</f>
+        <v>spw_link_connecting</v>
+      </c>
+      <c r="D29" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C29,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>1</v>
+      </c>
+      <c r="F29" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C29,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>9</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L29" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKSTAT_CONNECTING_MSK</v>
+      </c>
+      <c r="M29" s="32">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="O29" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKSTAT_CONNECTING_MSK  (1 &lt;&lt; 9)</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C30" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E9</f>
+        <v>spw_link_started</v>
+      </c>
+      <c r="D30" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C30,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>1</v>
+      </c>
+      <c r="F30" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C30,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>10</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L30" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKSTAT_STARTED_MSK</v>
+      </c>
+      <c r="M30" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O30" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKSTAT_STARTED_MSK     (1 &lt;&lt; 10)</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C31" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E11</f>
+        <v>spw_err_disconnect</v>
+      </c>
+      <c r="D31" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C31,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="32">
+        <v>1</v>
+      </c>
+      <c r="F31" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C31,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L31" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKERR_DISCONNECT_MSK</v>
+      </c>
+      <c r="M31" s="32">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="O31" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKERR_DISCONNECT_MSK   (1 &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C32" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E12</f>
+        <v>spw_err_parity</v>
+      </c>
+      <c r="D32" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C32,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C32,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>17</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L32" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKERR_PARITY_MSK</v>
+      </c>
+      <c r="M32" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O32" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKERR_PARITY_MSK       (1 &lt;&lt; 17)</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C33" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E13</f>
+        <v>spw_err_escape</v>
+      </c>
+      <c r="D33" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C33,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E33" s="32">
+        <v>1</v>
+      </c>
+      <c r="F33" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C33,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>18</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L33" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKERR_ESCAPE_MSK</v>
+      </c>
+      <c r="M33" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O33" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKERR_ESCAPE_MSK       (1 &lt;&lt; 18)</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C34" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E14</f>
+        <v>spw_err_credit</v>
+      </c>
+      <c r="D34" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C34,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E34" s="32">
+        <v>1</v>
+      </c>
+      <c r="F34" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C34,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>19</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L34" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKERR_CREDIT_MSK</v>
+      </c>
+      <c r="M34" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O34" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKERR_CREDIT_MSK       (1 &lt;&lt; 19)</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C35" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E16</f>
+        <v>spw_lnkcfg_txdivcnt</v>
+      </c>
+      <c r="D35" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C35,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="F35" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C35,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>24</v>
+      </c>
+      <c r="H35" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L35" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v>COMM_SPW_LNKCFG_TXDIVCNT_MSK</v>
+      </c>
+      <c r="M35" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O35" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_SPW_LNKCFG_TXDIVCNT_MSK     (0xFF &lt;&lt; 24)</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D36" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C36,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F36" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C36,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O36" s="62"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C37" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E17</f>
+        <v>timecode_time</v>
+      </c>
+      <c r="D37" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C37,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>6</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="F37" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C37,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="J37" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L37" s="32" t="str">
+        <f t="shared" ref="L37:L39" si="7">CONCATENATE(H37,I37,J37)</f>
+        <v>COMM_TIMECODE_TIME_MSK</v>
+      </c>
+      <c r="M37" s="32">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="O37" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_TIMECODE_TIME_MSK           (0b111111 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C38" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E18</f>
+        <v>timecode_control</v>
+      </c>
+      <c r="D38" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C38,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>2</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="F38" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C38,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>6</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L38" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>COMM_TIMECODE_CONTROL_MSK</v>
+      </c>
+      <c r="M38" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O38" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_TIMECODE_CONTROL_MSK        (0b11 &lt;&lt; 6)</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C39" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E19</f>
+        <v>timecode_clear</v>
+      </c>
+      <c r="D39" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C39,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E39" s="32">
+        <v>1</v>
+      </c>
+      <c r="F39" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C39,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="J39" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L39" s="32" t="str">
+        <f t="shared" si="7"/>
+        <v>COMM_TIMECODE_CLR_MSK</v>
+      </c>
+      <c r="M39" s="32">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="O39" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_TIMECODE_CLR_MSK            (1 &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D40" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C40,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F40" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C40,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O40" s="62"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C41" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E21</f>
+        <v>fee_machine_clear</v>
+      </c>
+      <c r="D41" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C41,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E41" s="32">
+        <v>1</v>
+      </c>
+      <c r="F41" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C41,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L41" s="32" t="str">
+        <f t="shared" ref="L41:L44" si="8">CONCATENATE(H41,I41,J41)</f>
+        <v>COMM_FEE_MACHINE_CLR_MSK</v>
+      </c>
+      <c r="M41" s="32">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="O41" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_FEE_MACHINE_CLR_MSK         (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C42" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E22</f>
+        <v>fee_machine_stop</v>
+      </c>
+      <c r="D42" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C42,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E42" s="32">
+        <v>1</v>
+      </c>
+      <c r="F42" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C42,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>1</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I42" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L42" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v>COMM_FEE_MACHINE_STOP_MSK</v>
+      </c>
+      <c r="M42" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O42" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_FEE_MACHINE_STOP_MSK        (1 &lt;&lt; 1)</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C43" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E23</f>
+        <v>fee_machine_start</v>
+      </c>
+      <c r="D43" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C43,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E43" s="32">
+        <v>1</v>
+      </c>
+      <c r="F43" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C43,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>2</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="J43" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L43" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v>COMM_FEE_MACHINE_START_MSK</v>
+      </c>
+      <c r="M43" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O43" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_FEE_MACHINE_START_MSK       (1 &lt;&lt; 2)</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C44" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E24</f>
+        <v>fee_masking_en</v>
+      </c>
+      <c r="D44" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C44,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="32">
+        <v>1</v>
+      </c>
+      <c r="F44" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C44,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>3</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L44" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v>COMM_FEE_MASKING_EN_MSK</v>
+      </c>
+      <c r="M44" s="32">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="O44" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_FEE_MASKING_EN_MSK          (1 &lt;&lt; 3)</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D45" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C45,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F45" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C45,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O45" s="62"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C46" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E26</f>
+        <v>windowing_right_buffer_empty</v>
+      </c>
+      <c r="D46" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C46,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E46" s="32">
+        <v>1</v>
+      </c>
+      <c r="F46" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C46,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="J46" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L46" s="32" t="str">
+        <f t="shared" ref="L46:L47" si="9">CONCATENATE(H46,I46,J46)</f>
+        <v>COMM_WIND_RIGH_BUFF_EMPTY_MSK</v>
+      </c>
+      <c r="M46" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O46" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_WIND_RIGH_BUFF_EMPTY_MSK    (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C47" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E27</f>
+        <v>windowing_left_buffer_empty</v>
+      </c>
+      <c r="D47" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C47,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E47" s="32">
+        <v>1</v>
+      </c>
+      <c r="F47" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C47,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="J47" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L47" s="32" t="str">
+        <f t="shared" si="9"/>
+        <v>COMM_WIND_LEFT_BUFF_EMPTY_MSK</v>
+      </c>
+      <c r="M47" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O47" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_WIND_LEFT_BUFF_EMPTY_MSK    (1 &lt;&lt; 1)</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D48" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C48,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F48" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C48,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O48" s="62"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C49" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E29</f>
+        <v>rmap_target_logical_addr</v>
+      </c>
+      <c r="D49" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C49,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="F49" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C49,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="J49" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L49" s="32" t="str">
+        <f t="shared" ref="L49:L50" si="10">CONCATENATE(H49,I49,J49)</f>
+        <v>COMM_RMAP_TARGET_LOG_ADDR_MSK</v>
+      </c>
+      <c r="M49" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O49" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_TARGET_LOG_ADDR_MSK    (0xFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C50" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E30</f>
+        <v>rmap_target_key</v>
+      </c>
+      <c r="D50" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C50,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="F50" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C50,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H50" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="J50" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L50" s="32" t="str">
+        <f t="shared" si="10"/>
+        <v>COMM_RMAP_TARGET_KEY_MSK</v>
+      </c>
+      <c r="M50" s="32">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="O50" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_TARGET_KEY_MSK         (0xFF &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D51" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C51,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F51" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C51,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O51" s="62"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C52" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E32</f>
+        <v>rmap_stat_command_received</v>
+      </c>
+      <c r="D52" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C52,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="32">
+        <v>1</v>
+      </c>
+      <c r="F52" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C52,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="J52" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L52" s="32" t="str">
+        <f t="shared" ref="L52:L65" si="11">CONCATENATE(H52,I52,J52)</f>
+        <v>COMM_RMAP_STAT_CMD_RECEIVED_MSK</v>
+      </c>
+      <c r="M52" s="32">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="O52" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_CMD_RECEIVED_MSK  (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C53" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E33</f>
+        <v>rmap_stat_write_requested</v>
+      </c>
+      <c r="D53" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C53,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E53" s="32">
+        <v>1</v>
+      </c>
+      <c r="F53" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C53,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>1</v>
+      </c>
+      <c r="H53" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="J53" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L53" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_WR_REQ_MSK</v>
+      </c>
+      <c r="M53" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O53" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_WR_REQ_MSK        (1 &lt;&lt; 1)</v>
+      </c>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C54" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E34</f>
+        <v>rmap_stat_write_authorized</v>
+      </c>
+      <c r="D54" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C54,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E54" s="32">
+        <v>1</v>
+      </c>
+      <c r="F54" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C54,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>2</v>
+      </c>
+      <c r="H54" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="J54" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L54" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_WR_AUTH_MSK</v>
+      </c>
+      <c r="M54" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O54" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_WR_AUTH_MSK       (1 &lt;&lt; 2)</v>
+      </c>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C55" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E35</f>
+        <v>rmap_stat_read_requested</v>
+      </c>
+      <c r="D55" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C55,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="32">
+        <v>1</v>
+      </c>
+      <c r="F55" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C55,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>3</v>
+      </c>
+      <c r="H55" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="J55" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L55" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_RD_REQ_MSK</v>
+      </c>
+      <c r="M55" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O55" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_RD_REQ_MSK        (1 &lt;&lt; 3)</v>
+      </c>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C56" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E36</f>
+        <v>rmap_stat_read_authorized</v>
+      </c>
+      <c r="D56" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C56,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E56" s="32">
+        <v>1</v>
+      </c>
+      <c r="F56" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C56,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>4</v>
+      </c>
+      <c r="H56" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="J56" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L56" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_RD_AUTH_MSK</v>
+      </c>
+      <c r="M56" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O56" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_RD_AUTH_MSK       (1 &lt;&lt; 4)</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C57" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E37</f>
+        <v>rmap_stat_reply_sended</v>
+      </c>
+      <c r="D57" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C57,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E57" s="32">
+        <v>1</v>
+      </c>
+      <c r="F57" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C57,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>5</v>
+      </c>
+      <c r="H57" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="J57" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L57" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_REPLY_SEND_MSK</v>
+      </c>
+      <c r="M57" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O57" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_REPLY_SEND_MSK    (1 &lt;&lt; 5)</v>
+      </c>
+    </row>
+    <row r="58" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C58" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E38</f>
+        <v>rmap_stat_discarded_package</v>
+      </c>
+      <c r="D58" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C58,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E58" s="32">
+        <v>1</v>
+      </c>
+      <c r="F58" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C58,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>6</v>
+      </c>
+      <c r="H58" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="J58" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L58" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_STAT_DISCARD_PKG_MSK</v>
+      </c>
+      <c r="M58" s="32">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="O58" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_STAT_DISCARD_PKG_MSK   (1 &lt;&lt; 6)</v>
+      </c>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C59" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E40</f>
+        <v>rmap_err_early_eop</v>
+      </c>
+      <c r="D59" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C59,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E59" s="32">
+        <v>1</v>
+      </c>
+      <c r="F59" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C59,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H59" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="J59" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L59" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_EARLY_EOP_MSK</v>
+      </c>
+      <c r="M59" s="32">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="O59" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_EARLY_EOP_MSK      (1 &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C60" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E41</f>
+        <v>rmap_err_eep</v>
+      </c>
+      <c r="D60" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C60,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E60" s="32">
+        <v>1</v>
+      </c>
+      <c r="F60" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C60,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>17</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I60" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="J60" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L60" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_EEP_MSK</v>
+      </c>
+      <c r="M60" s="32">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="O60" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_EEP_MSK            (1 &lt;&lt; 17)</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C61" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E42</f>
+        <v>rmap_err_header_crc</v>
+      </c>
+      <c r="D61" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C61,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E61" s="32">
+        <v>1</v>
+      </c>
+      <c r="F61" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C61,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>18</v>
+      </c>
+      <c r="H61" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="J61" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L61" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_HEADER_CRC_MSK</v>
+      </c>
+      <c r="M61" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O61" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_HEADER_CRC_MSK     (1 &lt;&lt; 18)</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C62" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E43</f>
+        <v>rmap_err_unused_packet_type</v>
+      </c>
+      <c r="D62" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C62,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E62" s="32">
+        <v>1</v>
+      </c>
+      <c r="F62" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C62,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>19</v>
+      </c>
+      <c r="H62" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="J62" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L62" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_UNUSED_PKT_MSK</v>
+      </c>
+      <c r="M62" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O62" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_UNUSED_PKT_MSK     (1 &lt;&lt; 19)</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C63" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E44</f>
+        <v>rmap_err_invalid_command_code</v>
+      </c>
+      <c r="D63" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C63,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E63" s="32">
+        <v>1</v>
+      </c>
+      <c r="F63" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C63,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>20</v>
+      </c>
+      <c r="H63" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I63" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="J63" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L63" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_INVALID_CMD_MSK</v>
+      </c>
+      <c r="M63" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O63" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_INVALID_CMD_MSK    (1 &lt;&lt; 20)</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C64" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E45</f>
+        <v>rmap_err_too_much_data</v>
+      </c>
+      <c r="D64" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C64,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="32">
+        <v>1</v>
+      </c>
+      <c r="F64" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C64,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>21</v>
+      </c>
+      <c r="H64" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I64" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="J64" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L64" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_TOO_MUCH_DATA_MSK</v>
+      </c>
+      <c r="M64" s="32">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="O64" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_TOO_MUCH_DATA_MSK  (1 &lt;&lt; 21)</v>
+      </c>
+    </row>
+    <row r="65" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C65" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E46</f>
+        <v>rmap_err_invalid_data_crc</v>
+      </c>
+      <c r="D65" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C65,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E65" s="32">
+        <v>1</v>
+      </c>
+      <c r="F65" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C65,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>22</v>
+      </c>
+      <c r="H65" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I65" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="J65" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L65" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>COMM_RMAP_ERR_INVALID_DCRC_MSK</v>
+      </c>
+      <c r="M65" s="32">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="O65" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_ERR_INVALID_DCRC_MSK   (1 &lt;&lt; 22)</v>
+      </c>
+    </row>
+    <row r="66" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D66" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C66,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F66" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C66,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O66" s="62"/>
+    </row>
+    <row r="67" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C67" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E48</f>
+        <v>rmap_last_write_addr</v>
+      </c>
+      <c r="D67" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C67,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>32</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="F67" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C67,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I67" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="J67" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L67" s="32" t="str">
+        <f t="shared" ref="L67" si="12">CONCATENATE(H67,I67,J67)</f>
+        <v>COMM_RMAP_LST_WR_ADDR_MSK</v>
+      </c>
+      <c r="M67" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O67" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_LST_WR_ADDR_MSK        (0xFFFFFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="68" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D68" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C68,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F68" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C68,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O68" s="62"/>
+    </row>
+    <row r="69" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C69" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E49</f>
+        <v>rmap_last_read_addr</v>
+      </c>
+      <c r="D69" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C69,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>32</v>
+      </c>
+      <c r="E69" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="F69" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C69,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I69" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J69" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L69" s="32" t="str">
+        <f t="shared" ref="L69" si="13">CONCATENATE(H69,I69,J69)</f>
+        <v>COMM_RMAP_LST_RD_ADDR_MSK</v>
+      </c>
+      <c r="M69" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O69" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_RMAP_LST_RD_ADDR_MSK        (0xFFFFFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="70" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D70" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C70,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F70" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C70,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O70" s="62"/>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C71" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E50</f>
+        <v>data_pkt_ccd_x_size</v>
+      </c>
+      <c r="D71" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C71,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E71" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F71" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C71,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I71" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="J71" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L71" s="32" t="str">
+        <f t="shared" ref="L71:L72" si="14">CONCATENATE(H71,I71,J71)</f>
+        <v>COMM_DATA_PKT_CCD_X_SIZE_MSK</v>
+      </c>
+      <c r="M71" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O71" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_CCD_X_SIZE_MSK     (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="72" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C72" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E51</f>
+        <v>data_pkt_ccd_y_size</v>
+      </c>
+      <c r="D72" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C72,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E72" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F72" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C72,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H72" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I72" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="J72" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L72" s="32" t="str">
+        <f t="shared" si="14"/>
+        <v>COMM_DATA_PKT_CCD_Y_SIZE_MSK</v>
+      </c>
+      <c r="M72" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O72" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_CCD_Y_SIZE_MSK     (0xFFFF &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="73" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D73" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C73,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F73" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C73,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O73" s="62"/>
+    </row>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C74" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E52</f>
+        <v>data_pkt_data_y_size</v>
+      </c>
+      <c r="D74" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C74,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E74" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F74" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C74,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H74" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I74" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="J74" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L74" s="32" t="str">
+        <f t="shared" ref="L74:L75" si="15">CONCATENATE(H74,I74,J74)</f>
+        <v>COMM_DATA_PKT_DATA_Y_SIZE_MSK</v>
+      </c>
+      <c r="M74" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O74" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_DATA_Y_SIZE_MSK    (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="75" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C75" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E53</f>
+        <v>data_pkt_overscan_y_size</v>
+      </c>
+      <c r="D75" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C75,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E75" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F75" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C75,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H75" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I75" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="J75" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L75" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>COMM_DATA_PKT_OVER_Y_SIZE_MSK</v>
+      </c>
+      <c r="M75" s="32">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="O75" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_OVER_Y_SIZE_MSK    (0xFFFF &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="76" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D76" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C76,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F76" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C76,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O76" s="62"/>
+    </row>
+    <row r="77" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C77" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E54</f>
+        <v>data_pkt_packet_length</v>
+      </c>
+      <c r="D77" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C77,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E77" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F77" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C77,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H77" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I77" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="J77" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L77" s="32" t="str">
+        <f t="shared" ref="L77" si="16">CONCATENATE(H77,I77,J77)</f>
+        <v>COMM_DATA_PKT_LENGTH_MSK</v>
+      </c>
+      <c r="M77" s="32">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="O77" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_LENGTH_MSK         (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="78" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D78" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C78,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F78" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C78,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O78" s="62"/>
+    </row>
+    <row r="79" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C79" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E56</f>
+        <v>data_pkt_fee_mode</v>
+      </c>
+      <c r="D79" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C79,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="F79" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C79,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H79" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I79" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="J79" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L79" s="32" t="str">
+        <f t="shared" ref="L79:L80" si="17">CONCATENATE(H79,I79,J79)</f>
+        <v>COMM_DATA_PKT_FEE_MODE_MSK</v>
+      </c>
+      <c r="M79" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O79" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_FEE_MODE_MSK       (0xFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="80" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C80" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E57</f>
+        <v>data_pkt_ccd_number</v>
+      </c>
+      <c r="D80" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C80,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="F80" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C80,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H80" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I80" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="J80" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L80" s="32" t="str">
+        <f t="shared" si="17"/>
+        <v>COMM_DATA_PKT_CCD_NUMBER_MSK</v>
+      </c>
+      <c r="M80" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O80" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_CCD_NUMBER_MSK     (0xFF &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="81" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D81" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C81,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F81" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C81,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O81" s="62"/>
+    </row>
+    <row r="82" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C82" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E59</f>
+        <v>data_pkt_header_length</v>
+      </c>
+      <c r="D82" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C82,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E82" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F82" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C82,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H82" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I82" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="J82" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L82" s="32" t="str">
+        <f t="shared" ref="L82:L83" si="18">CONCATENATE(H82,I82,J82)</f>
+        <v>COMM_DATA_PKT_HDR_LENGTH_MSK</v>
+      </c>
+      <c r="M82" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O82" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_HDR_LENGTH_MSK     (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="83" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C83" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E60</f>
+        <v>data_pkt_header_type</v>
+      </c>
+      <c r="D83" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C83,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E83" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F83" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C83,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H83" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I83" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="J83" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L83" s="32" t="str">
+        <f t="shared" si="18"/>
+        <v>COMM_DATA_PKT_HDR_TYPE_MSK</v>
+      </c>
+      <c r="M83" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O83" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_HDR_TYPE_MSK       (0xFFFF &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="84" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D84" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C84,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F84" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C84,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O84" s="62"/>
+    </row>
+    <row r="85" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C85" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E61</f>
+        <v>data_pkt_header_frame_counter</v>
+      </c>
+      <c r="D85" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C85,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F85" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C85,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H85" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I85" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="J85" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L85" s="32" t="str">
+        <f t="shared" ref="L85:L86" si="19">CONCATENATE(H85,I85,J85)</f>
+        <v>COMM_DATA_PKT_HDR_FRAME_CNT_MSK</v>
+      </c>
+      <c r="M85" s="32">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="O85" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_HDR_FRAME_CNT_MSK  (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="86" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C86" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E62</f>
+        <v>data_pkt_header_sequence_counter</v>
+      </c>
+      <c r="D86" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C86,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E86" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F86" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C86,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H86" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I86" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="J86" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L86" s="32" t="str">
+        <f t="shared" si="19"/>
+        <v>COMM_DATA_PKT_SEQ_CNT_MSK</v>
+      </c>
+      <c r="M86" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O86" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_SEQ_CNT_MSK        (0xFFFF &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="87" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D87" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C87,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F87" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C87,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O87" s="62"/>
+    </row>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C88" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E63</f>
+        <v>data_pkt_line_delay</v>
+      </c>
+      <c r="D88" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C88,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E88" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F88" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C88,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H88" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I88" s="32" t="s">
+        <v>347</v>
+      </c>
+      <c r="J88" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L88" s="32" t="str">
+        <f t="shared" ref="L88" si="20">CONCATENATE(H88,I88,J88)</f>
+        <v>COMM_DATA_PKT_LINE_DLY_MSK</v>
+      </c>
+      <c r="M88" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O88" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_LINE_DLY_MSK       (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="89" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D89" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C89,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F89" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C89,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O89" s="62"/>
+    </row>
+    <row r="90" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C90" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E65</f>
+        <v>data_pkt_column_delay</v>
+      </c>
+      <c r="D90" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C90,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E90" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F90" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C90,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H90" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I90" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="J90" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L90" s="32" t="str">
+        <f t="shared" ref="L90" si="21">CONCATENATE(H90,I90,J90)</f>
+        <v>COMM_DATA_PKT_COLUMN_DLY_MSK</v>
+      </c>
+      <c r="M90" s="32">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="O90" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_COLUMN_DLY_MSK     (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="91" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D91" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C91,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F91" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C91,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O91" s="62"/>
+    </row>
+    <row r="92" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C92" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E67</f>
+        <v>data_pkt_adc_delay</v>
+      </c>
+      <c r="D92" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C92,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="E92" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="F92" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C92,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H92" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I92" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="J92" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L92" s="32" t="str">
+        <f t="shared" ref="L92" si="22">CONCATENATE(H92,I92,J92)</f>
+        <v>COMM_DATA_PKT_ADC_DLY_MSK</v>
+      </c>
+      <c r="M92" s="32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O92" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_DATA_PKT_ADC_DLY_MSK        (0xFFFF &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="93" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D93" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C93,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F93" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C93,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O93" s="62"/>
+    </row>
+    <row r="94" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C94" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E69</f>
+        <v>comm_rmap_write_command_en</v>
+      </c>
+      <c r="D94" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C94,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E94" s="32">
+        <v>1</v>
+      </c>
+      <c r="F94" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C94,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H94" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I94" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="J94" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L94" s="32" t="str">
+        <f t="shared" ref="L94:L97" si="23">CONCATENATE(H94,I94,J94)</f>
+        <v>COMM_IRQ_RMAP_WRCMD_EN_MSK</v>
+      </c>
+      <c r="M94" s="32">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="O94" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v>#define COMM_IRQ_RMAP_WRCMD_EN_MSK       (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="95" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C95" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E71</f>
+        <v>comm_right_buffer_empty_en</v>
+      </c>
+      <c r="D95" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C95,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E95" s="32">
+        <v>1</v>
+      </c>
+      <c r="F95" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C95,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H95" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I95" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="J95" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L95" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>COMM_IRQ_RIGH_BUFF_EPY_EN_MSK</v>
+      </c>
+      <c r="M95" s="32">
+        <f t="shared" ref="M95:M97" si="24">LEN(L95)</f>
+        <v>29</v>
+      </c>
+      <c r="O95" s="62" t="str">
+        <f t="shared" ref="O95:O97" si="25">CONCATENATE("#define ",L95, REPT(" ",32 - LEN(L95))," ","(", E95," &lt;&lt; ", F95,")")</f>
+        <v>#define COMM_IRQ_RIGH_BUFF_EPY_EN_MSK    (1 &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="96" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C96" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E72</f>
+        <v>comm_left_buffer_empty_en</v>
+      </c>
+      <c r="D96" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C96,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E96" s="32">
+        <v>1</v>
+      </c>
+      <c r="F96" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C96,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>9</v>
+      </c>
+      <c r="H96" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I96" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="J96" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L96" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>COMM_IRQ_LEFT_BUFF_EPY_EN_MSK</v>
+      </c>
+      <c r="M96" s="32">
+        <f t="shared" si="24"/>
+        <v>29</v>
+      </c>
+      <c r="O96" s="62" t="str">
+        <f t="shared" si="25"/>
+        <v>#define COMM_IRQ_LEFT_BUFF_EPY_EN_MSK    (1 &lt;&lt; 9)</v>
+      </c>
+    </row>
+    <row r="97" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C97" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E74</f>
+        <v>comm_global_irq_en</v>
+      </c>
+      <c r="D97" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C97,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E97" s="32">
+        <v>1</v>
+      </c>
+      <c r="F97" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C97,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>16</v>
+      </c>
+      <c r="H97" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I97" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="J97" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L97" s="32" t="str">
+        <f t="shared" si="23"/>
+        <v>COMM_IRQ_GLOBAL_EN_MSK</v>
+      </c>
+      <c r="M97" s="32">
+        <f t="shared" si="24"/>
+        <v>22</v>
+      </c>
+      <c r="O97" s="62" t="str">
+        <f t="shared" si="25"/>
+        <v>#define COMM_IRQ_GLOBAL_EN_MSK           (1 &lt;&lt; 16)</v>
+      </c>
+    </row>
+    <row r="98" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D98" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C98,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F98" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C98,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O98" s="62"/>
+    </row>
+    <row r="99" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C99" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E76</f>
+        <v>comm_rmap_write_command_flag</v>
+      </c>
+      <c r="D99" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C99,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E99" s="32">
+        <v>1</v>
+      </c>
+      <c r="F99" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C99,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H99" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I99" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="J99" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L99" s="32" t="str">
+        <f t="shared" ref="L99:L100" si="26">CONCATENATE(H99,I99,J99)</f>
+        <v>COMM_IRQ_RMAP_WRCMD_FLG_MSK</v>
+      </c>
+      <c r="M99" s="32">
+        <f t="shared" ref="M99:M100" si="27">LEN(L99)</f>
+        <v>27</v>
+      </c>
+      <c r="O99" s="62" t="str">
+        <f t="shared" ref="O99:O103" si="28">CONCATENATE("#define ",L99, REPT(" ",32 - LEN(L99))," ","(", E99," &lt;&lt; ", F99,")")</f>
+        <v>#define COMM_IRQ_RMAP_WRCMD_FLG_MSK      (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="100" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C100" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E78</f>
+        <v>comm_buffer_empty_flag</v>
+      </c>
+      <c r="D100" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C100,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E100" s="32">
+        <v>1</v>
+      </c>
+      <c r="F100" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C100,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H100" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I100" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="J100" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L100" s="32" t="str">
+        <f t="shared" si="26"/>
+        <v>COMM_IRQ_BUFF_EPY_FLG_MSK</v>
+      </c>
+      <c r="M100" s="32">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="O100" s="62" t="str">
+        <f t="shared" si="28"/>
+        <v>#define COMM_IRQ_BUFF_EPY_FLG_MSK        (1 &lt;&lt; 8)</v>
+      </c>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D101" s="32" t="str">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C101,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v/>
+      </c>
+      <c r="F101" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C101,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v/>
+      </c>
+      <c r="O101" s="62"/>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C102" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E80</f>
+        <v>comm_rmap_write_command_flag_clear</v>
+      </c>
+      <c r="D102" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C102,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E102" s="32">
+        <v>1</v>
+      </c>
+      <c r="F102" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C102,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="H102" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I102" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="J102" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L102" s="32" t="str">
+        <f t="shared" ref="L102:L103" si="29">CONCATENATE(H102,I102,J102)</f>
+        <v>COMM_IRQ_RMAP_WRCMD_FLG_CLR_MSK</v>
+      </c>
+      <c r="M102" s="32">
+        <f t="shared" ref="M102:M103" si="30">LEN(L102)</f>
+        <v>31</v>
+      </c>
+      <c r="O102" s="62" t="str">
+        <f t="shared" si="28"/>
+        <v>#define COMM_IRQ_RMAP_WRCMD_FLG_CLR_MSK  (1 &lt;&lt; 0)</v>
+      </c>
+    </row>
+    <row r="103" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C103" s="32" t="str">
+        <f>'AVS COMM Registers TABLE'!E82</f>
+        <v>comm_buffer_empty_flag_clear</v>
+      </c>
+      <c r="D103" s="32">
+        <f>_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$K$2:$K$83,MATCH('NIOS defines'!C103,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E103" s="32">
+        <v>1</v>
+      </c>
+      <c r="F103" s="32" t="str">
+        <f>TEXT(RIGHT(_xlfn.IFNA(INDEX('AVS COMM Registers TABLE'!$J$2:$J$83,MATCH('NIOS defines'!C103,'AVS COMM Registers TABLE'!$E$2:$E$83,0)),""),2),"0")</f>
+        <v>8</v>
+      </c>
+      <c r="H103" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="I103" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="J103" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="L103" s="32" t="str">
+        <f t="shared" si="29"/>
+        <v>COMM_IRQ_BUFF_EPY_FLG_CLR_MSK</v>
+      </c>
+      <c r="M103" s="32">
+        <f t="shared" si="30"/>
+        <v>29</v>
+      </c>
+      <c r="O103" s="62" t="str">
+        <f t="shared" si="28"/>
+        <v>#define COMM_IRQ_BUFF_EPY_FLG_CLR_MSK    (1 &lt;&lt; 8)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P158"/>
@@ -26695,7 +30193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:E62"/>
   <sheetViews>
@@ -27809,12 +31307,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
@@ -33864,12 +37362,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AB95"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>